<commit_message>
update the final results table, again
</commit_message>
<xml_diff>
--- a/results/final_scores.xlsx
+++ b/results/final_scores.xlsx
@@ -505,12 +505,12 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Working training code for murmur task?</t>
+          <t>Robust training code for murmur task?</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Working training code for clinical outcome task?</t>
+          <t>Robust training code for clinical outcome task?</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">

</xml_diff>